<commit_message>
renamed jobboard_instanes to jobboard_list
</commit_message>
<xml_diff>
--- a/job_files/jobboard_info.xlsx
+++ b/job_files/jobboard_info.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\github\job_visitor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\github\job_visitor\job_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75020AEC-DD6A-472E-BA1A-C186C99D008D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26ED663A-C81D-49D6-957D-4866141E9C99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3001,7 +3001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="405" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -3257,7 +3257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
added example usage to readme, updated table
</commit_message>
<xml_diff>
--- a/job_files/jobboard_info.xlsx
+++ b/job_files/jobboard_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jai\Documents\github\job_visitor\job_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC8EECBE-83B9-4519-9500-56252C3DB994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEC319F-29F5-460D-9D24-4BB922C70F99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="325">
   <si>
     <t>name</t>
   </si>
@@ -65,10 +65,6 @@
   <si>
     <t>https://philanthropynewsdigest.org/jobs/(search)/?attr_tags_org_type_lk%5B%5D=&amp;attr_tags_job_type_lk%5B%5D=research%2Fpolicy&amp;attr_tags_location_lk%5B%5D=&amp;search_text=&amp;btn=&amp;day_filter=0
 https://philanthropynewsdigest.org/jobs/(search)/?attr_tags_org_type_lk%5B%5D=&amp;attr_tags_job_type_lk%5B%5D=consultant&amp;attr_tags_location_lk%5B%5D=&amp;search_text=&amp;btn=&amp;day_filter=0</t>
-  </si>
-  <si>
-    <t>https://www.devex.com/jobs/search?filter%5Bjob_types%5D%5B%5D=community%20jobs&amp;filter%5Blocations%5D%5B%5D=United%20States&amp;filter%5Bkeywords%5D%5B%5D=Data&amp;filter%5Bis_featured%5D=false&amp;page%5Bnumber%5D=3&amp;sorting%5Border%5D=desc&amp;sorting%5Bfield%5D=updated_at
-https://www.devex.com/jobs/search?filter%5Bjob_types%5D%5B%5D=community%20jobs&amp;filter%5Blocations%5D%5B%5D=United%20States&amp;filter%5Bkeywords%5D%5B%5D=Evaluation&amp;filter%5Bis_featured%5D=false&amp;sorting%5Border%5D=desc&amp;sorting%5Bfield%5D=updated_at</t>
   </si>
   <si>
     <t>https://www.foundationlist.org/jobs/advanced-search/?query=Data&amp;location=California&amp;results=1</t>
@@ -946,13 +942,116 @@
   <si>
     <t>The Modern Classrooms Project empowers educators to meet every student’s needs through blended, self-paced, mastery-based instruction. 
 We lead a movement of educators in implementing a research-backed instructional model that leverages technology to improve educator effectiveness and learner understanding.</t>
+  </si>
+  <si>
+    <t>https://www.ussif.org/jobs_search.asp?proc=y</t>
+  </si>
+  <si>
+    <t>US SIF: The Forum for Sustainable and Responsible Investment</t>
+  </si>
+  <si>
+    <t>the leading voice advancing sustainable investing across all asset classes. Its mission is to rapidly shift investment practices toward sustainability, focusing on long-term investment and the generation of positive social and environmental impacts.</t>
+  </si>
+  <si>
+    <t>https://acumen.org/work-with-us/</t>
+  </si>
+  <si>
+    <t>Impact investing - Neither the markets nor aid alone can solve the problems of poverty. More than two billion people around the world lack access to basic goods and services—from clean water and electricity to an education and the freedom to participate in the economy. We’re here to change that. Our vision is a world based on dignity, where every human being has the same opportunity. Rather than giving philanthropy away, we invest it in companies and change makers.</t>
+  </si>
+  <si>
+    <t>https://change-finance.com/careers/</t>
+  </si>
+  <si>
+    <t>Change Finance</t>
+  </si>
+  <si>
+    <t>Change Finance builds performance-oriented investment products for the sustainability-minded investor. We believe investing for good can profit people, planet, and investors. Through a conscious, rigorous, rules-based approach, we’ve created an Enhanced ESG methodology that underpins our investment products.</t>
+  </si>
+  <si>
+    <t>TransformEd</t>
+  </si>
+  <si>
+    <t>https://www.transformingeducation.org/get-involved/careers/</t>
+  </si>
+  <si>
+    <t>At TransformEd, we believe that every young person deserves to be supported in the development of their whole self, yet, due to systemic oppression, students from historically marginalized populations often do not have the access they deserve to rich, positive learning environments that foster their development. We believe that the education system is ripe for transformation, to better serve the needs of students, families, and communities. We focus on the school system as the unit of change, partnering directly with school districts and other education support organizations in order to support educators and leaders in changing policies and practices to foster whole child development.</t>
+  </si>
+  <si>
+    <t>Harvard</t>
+  </si>
+  <si>
+    <t>https://sjobs.brassring.com/TGnewUI/Search/Home/Home?partnerid=25240&amp;siteid=5341#keyWordSearch=Python</t>
+  </si>
+  <si>
+    <t>I was recently invited to interview for a research specialist position with Harvard that matches my open-source &amp; data analytic contributions/intersts. I've decided that higher education is a good opportunity to contribute to exciting, meaningful projects, develop new skills, and network</t>
+  </si>
+  <si>
+    <t>Yale</t>
+  </si>
+  <si>
+    <t>https://sjobs.brassring.com/TGnewUI/Search/Home/Home?partnerid=25053&amp;siteid=5248#keyWordSearch=Evaluation</t>
+  </si>
+  <si>
+    <t>MIT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://careers.peopleclick.com/careerscp/client_mit/external/search/search.html
+</t>
+  </si>
+  <si>
+    <t>Princeton</t>
+  </si>
+  <si>
+    <t>https://hub-princeton.icims.com/jobs/search?ss=1&amp;hashed=-435679187&amp;mobile=false&amp;width=1200&amp;height=500&amp;bga=true&amp;needsRedirect=false&amp;jan1offset=-300&amp;jun1offset=-240</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>https://careersearch.stanford.edu/jobs/search/6371937
+https://careersearch.stanford.edu/jobs/search/6371888
+https://careersearch.stanford.edu/jobs/search/6371903
+https://careersearch.stanford.edu/jobs/search/6371904</t>
+  </si>
+  <si>
+    <t>Progressive Exchange</t>
+  </si>
+  <si>
+    <t>The Progressive Exchange is an online community that was started in 2004 by M+R as a way to share information about online strategies, tactics and tools among people doing internet organizing, advocacy, marketing and fundraising on behalf of the public interest.</t>
+  </si>
+  <si>
+    <t>https://www.progressiveexchange.org/vb/forumdisplay.php?f=35</t>
+  </si>
+  <si>
+    <t>Jobs that are left</t>
+  </si>
+  <si>
+    <t>https://groups.google.com/g/jobsleft
+https://groups.google.com/g/jobsleft</t>
+  </si>
+  <si>
+    <r>
+      <t>obs That Are Left</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4D5156"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (JTAL) is a popular google group for the Democratic and Progressive community managed by GAIN POWER. Questions about our policies ...</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.devex.com/jobs/search?filter%5Blocations%5D%5B%5D=United%20States&amp;filter%5Bis_featured%5D=false&amp;sorting%5Border%5D=desc&amp;sorting%5Bfield%5D=_score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -967,6 +1066,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4D5156"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -989,13 +1094,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1276,11 +1379,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L89"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1295,38 +1398,39 @@
     <col min="8" max="8" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1334,13 +1438,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E2" s="1">
         <v>6</v>
@@ -1366,13 +1470,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E3" s="1">
         <v>6</v>
@@ -1398,13 +1502,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1">
         <v>40</v>
@@ -1430,13 +1534,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="1">
         <v>40</v>
@@ -1451,10 +1555,10 @@
         <v>1</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1462,13 +1566,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E6" s="1">
         <v>6</v>
@@ -1494,13 +1598,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="1">
         <v>40</v>
@@ -1526,13 +1630,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E8" s="1">
         <v>40</v>
@@ -1558,13 +1662,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E9" s="1">
         <v>6</v>
@@ -1590,13 +1694,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" s="1">
         <v>40</v>
@@ -1611,10 +1715,10 @@
         <v>1</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1622,13 +1726,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E11" s="1">
         <v>6</v>
@@ -1654,13 +1758,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E12" s="1">
         <v>6</v>
@@ -1686,13 +1790,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" s="1">
         <v>40</v>
@@ -1707,10 +1811,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1718,13 +1822,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E14" s="1">
         <v>5</v>
@@ -1750,13 +1854,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>324</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E15" s="1">
         <v>6</v>
@@ -1782,13 +1886,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E16" s="1">
         <v>40</v>
@@ -1814,13 +1918,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E17" s="1">
         <v>5</v>
@@ -1846,13 +1950,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E18" s="1">
         <v>40</v>
@@ -1878,13 +1982,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E19" s="1">
         <v>40</v>
@@ -1899,10 +2003,10 @@
         <v>1</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1910,13 +2014,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>18</v>
+        <v>58</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E20" s="1">
         <v>5</v>
@@ -1942,13 +2046,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E21" s="1">
         <v>6</v>
@@ -1974,13 +2078,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E22" s="1">
         <v>40</v>
@@ -2006,13 +2110,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E23" s="1">
         <v>5</v>
@@ -2038,13 +2142,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E24" s="1">
         <v>11</v>
@@ -2070,13 +2174,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E25" s="1">
         <v>6</v>
@@ -2102,13 +2206,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E26" s="1">
         <v>40</v>
@@ -2134,13 +2238,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E27" s="1">
         <v>6</v>
@@ -2166,13 +2270,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>193</v>
+        <v>65</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E28" s="1">
         <v>6</v>
@@ -2198,13 +2302,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>253</v>
+        <v>66</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E29" s="1">
         <v>2</v>
@@ -2230,13 +2334,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E30" s="1">
         <v>5</v>
@@ -2262,13 +2366,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E31" s="1">
         <v>40</v>
@@ -2283,10 +2387,10 @@
         <v>1</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -2294,13 +2398,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E32" s="1">
         <v>6</v>
@@ -2326,13 +2430,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E33" s="1">
         <v>6</v>
@@ -2358,13 +2462,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E34" s="1">
         <v>6</v>
@@ -2390,13 +2494,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E35" s="1">
         <v>6</v>
@@ -2422,13 +2526,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E36" s="1">
         <v>3</v>
@@ -2454,13 +2558,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E37" s="1">
         <v>40</v>
@@ -2486,13 +2590,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>249</v>
+        <v>75</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E38" s="1">
         <v>40</v>
@@ -2507,10 +2611,10 @@
         <v>1</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -2518,13 +2622,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>250</v>
+        <v>76</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E39" s="1">
         <v>40</v>
@@ -2550,13 +2654,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E40" s="1">
         <v>40</v>
@@ -2568,13 +2672,13 @@
         <v>1</v>
       </c>
       <c r="H40" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="J40" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
@@ -2582,13 +2686,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E41" s="1">
         <v>40</v>
@@ -2603,10 +2707,10 @@
         <v>1</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
@@ -2614,13 +2718,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E42" s="1">
         <v>40</v>
@@ -2646,13 +2750,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E43" s="1">
         <v>40</v>
@@ -2678,13 +2782,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E44" s="1">
         <v>40</v>
@@ -2710,13 +2814,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E45" s="1">
         <v>9</v>
@@ -2742,13 +2846,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E46" s="1">
         <v>9</v>
@@ -2774,13 +2878,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E47" s="1">
         <v>15</v>
@@ -2806,13 +2910,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E48" s="1">
         <v>40</v>
@@ -2838,13 +2942,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="E49" s="1">
         <v>40</v>
@@ -2870,13 +2974,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="E50" s="1">
         <v>40</v>
@@ -2902,13 +3006,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="E51" s="1">
         <v>40</v>
@@ -2934,13 +3038,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="E52" s="1">
         <v>40</v>
@@ -2966,13 +3070,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="D53" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="E53" s="1">
         <v>40</v>
@@ -2987,10 +3091,10 @@
         <v>1</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -2998,13 +3102,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C54" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="E54" s="1">
         <v>10</v>
@@ -3030,13 +3134,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>208</v>
       </c>
       <c r="E55" s="1">
         <v>40</v>
@@ -3062,13 +3166,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>211</v>
-      </c>
       <c r="D56" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E56" s="1">
         <v>40</v>
@@ -3094,13 +3198,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="D57" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="E57" s="1">
         <v>40</v>
@@ -3126,13 +3230,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="D58" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>217</v>
       </c>
       <c r="E58" s="1">
         <v>60</v>
@@ -3158,13 +3262,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="D59" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="E59" s="1">
         <v>40</v>
@@ -3190,13 +3294,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="D60" s="1" t="s">
         <v>222</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>223</v>
       </c>
       <c r="E60" s="1">
         <v>15</v>
@@ -3222,13 +3326,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>225</v>
       </c>
       <c r="E61" s="1">
         <v>15</v>
@@ -3243,7 +3347,7 @@
         <v>1</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J61" s="1">
         <v>0</v>
@@ -3254,13 +3358,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>228</v>
-      </c>
       <c r="D62" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E62" s="1">
         <v>10</v>
@@ -3286,13 +3390,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="E63" s="1">
         <v>10</v>
@@ -3318,13 +3422,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C64" s="1" t="s">
+      <c r="D64" s="1" t="s">
         <v>233</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>234</v>
       </c>
       <c r="E64" s="1">
         <v>10</v>
@@ -3345,18 +3449,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>236</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>237</v>
       </c>
       <c r="E65" s="1">
         <v>40</v>
@@ -3377,18 +3481,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="D66" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="E66" s="1">
         <v>40</v>
@@ -3409,18 +3513,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>243</v>
-      </c>
       <c r="D67" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E67" s="1">
         <v>60</v>
@@ -3441,18 +3545,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="D68" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="E68" s="1">
         <v>40</v>
@@ -3467,24 +3571,24 @@
         <v>1</v>
       </c>
       <c r="I68" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="J68" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="J68" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E69" s="1">
         <v>40</v>
@@ -3505,18 +3609,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="C70" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="E70" s="1">
         <v>40</v>
@@ -3537,18 +3641,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="D71" s="1" t="s">
         <v>261</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="E71" s="1">
         <v>40</v>
@@ -3569,18 +3673,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C72" s="5" t="s">
+      <c r="D72" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="E72" s="1">
         <v>10</v>
@@ -3601,18 +3705,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="C73" s="1" t="s">
+      <c r="D73" s="1" t="s">
         <v>267</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>268</v>
       </c>
       <c r="E73" s="1">
         <v>10</v>
@@ -3633,18 +3737,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="D74" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="E74" s="1">
         <v>10</v>
@@ -3664,21 +3768,19 @@
       <c r="J74" s="1">
         <v>8</v>
       </c>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>275</v>
       </c>
       <c r="E75" s="1">
         <v>60</v>
@@ -3698,21 +3800,19 @@
       <c r="J75" s="1">
         <v>8</v>
       </c>
-      <c r="K75" s="1"/>
-      <c r="L75" s="1"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>277</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>278</v>
       </c>
       <c r="E76" s="1">
         <v>60</v>
@@ -3732,21 +3832,19 @@
       <c r="J76" s="1">
         <v>8</v>
       </c>
-      <c r="K76" s="1"/>
-      <c r="L76" s="1"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="D77" s="1" t="s">
         <v>280</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>281</v>
       </c>
       <c r="E77" s="1">
         <v>60</v>
@@ -3766,21 +3864,19 @@
       <c r="J77" s="1">
         <v>8</v>
       </c>
-      <c r="K77" s="1"/>
-      <c r="L77" s="1"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>283</v>
       </c>
       <c r="E78" s="1">
         <v>60</v>
@@ -3800,21 +3896,19 @@
       <c r="J78" s="1">
         <v>8</v>
       </c>
-      <c r="K78" s="1"/>
-      <c r="L78" s="1"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="E79" s="1">
         <v>60</v>
@@ -3834,21 +3928,19 @@
       <c r="J79" s="1">
         <v>8</v>
       </c>
-      <c r="K79" s="1"/>
-      <c r="L79" s="1"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="C80" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>289</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>290</v>
       </c>
       <c r="E80" s="1">
         <v>60</v>
@@ -3868,21 +3960,19 @@
       <c r="J80" s="1">
         <v>8</v>
       </c>
-      <c r="K80" s="1"/>
-      <c r="L80" s="1"/>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="E81" s="1">
         <v>60</v>
@@ -3902,21 +3992,19 @@
       <c r="J81" s="1">
         <v>8</v>
       </c>
-      <c r="K81" s="1"/>
-      <c r="L81" s="1"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="C82" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>295</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>296</v>
       </c>
       <c r="E82" s="1">
         <v>60</v>
@@ -3936,36 +4024,358 @@
       <c r="J82" s="1">
         <v>8</v>
       </c>
-      <c r="K82" s="1"/>
-      <c r="L82" s="1"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K83" s="1"/>
-      <c r="L83" s="1"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K84" s="1"/>
-      <c r="L84" s="1"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K85" s="1"/>
-      <c r="L85" s="1"/>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K86" s="1"/>
-      <c r="L86" s="1"/>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K87" s="1"/>
-      <c r="L87" s="1"/>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K88" s="1"/>
-      <c r="L88" s="1"/>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K89" s="1"/>
-      <c r="L89" s="1"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E83" s="1">
+        <v>60</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0</v>
+      </c>
+      <c r="G83" s="1">
+        <v>1</v>
+      </c>
+      <c r="H83" s="1">
+        <v>1</v>
+      </c>
+      <c r="I83" s="1">
+        <v>2</v>
+      </c>
+      <c r="J83" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="E84" s="1">
+        <v>60</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0</v>
+      </c>
+      <c r="G84" s="1">
+        <v>1</v>
+      </c>
+      <c r="H84" s="1">
+        <v>0</v>
+      </c>
+      <c r="I84" s="1">
+        <v>0</v>
+      </c>
+      <c r="J84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="E85" s="1">
+        <v>60</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0</v>
+      </c>
+      <c r="G85" s="1">
+        <v>1</v>
+      </c>
+      <c r="H85" s="1">
+        <v>0</v>
+      </c>
+      <c r="I85" s="1">
+        <v>0</v>
+      </c>
+      <c r="J85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="E86" s="1">
+        <v>60</v>
+      </c>
+      <c r="F86" s="1">
+        <v>0</v>
+      </c>
+      <c r="G86" s="1">
+        <v>1</v>
+      </c>
+      <c r="H86" s="1">
+        <v>0</v>
+      </c>
+      <c r="I86" s="1">
+        <v>0</v>
+      </c>
+      <c r="J86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E87" s="1">
+        <v>60</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0</v>
+      </c>
+      <c r="G87" s="1">
+        <v>1</v>
+      </c>
+      <c r="H87" s="1">
+        <v>0</v>
+      </c>
+      <c r="I87" s="1">
+        <v>0</v>
+      </c>
+      <c r="J87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E88" s="1">
+        <v>60</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0</v>
+      </c>
+      <c r="G88" s="1">
+        <v>1</v>
+      </c>
+      <c r="H88" s="1">
+        <v>0</v>
+      </c>
+      <c r="I88" s="1">
+        <v>0</v>
+      </c>
+      <c r="J88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E89" s="1">
+        <v>60</v>
+      </c>
+      <c r="F89" s="1">
+        <v>0</v>
+      </c>
+      <c r="G89" s="1">
+        <v>1</v>
+      </c>
+      <c r="H89" s="1">
+        <v>0</v>
+      </c>
+      <c r="I89" s="1">
+        <v>0</v>
+      </c>
+      <c r="J89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E90" s="1">
+        <v>60</v>
+      </c>
+      <c r="F90" s="1">
+        <v>0</v>
+      </c>
+      <c r="G90" s="1">
+        <v>1</v>
+      </c>
+      <c r="H90" s="1">
+        <v>0</v>
+      </c>
+      <c r="I90" s="1">
+        <v>0</v>
+      </c>
+      <c r="J90" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E91" s="1">
+        <v>60</v>
+      </c>
+      <c r="F91" s="1">
+        <v>0</v>
+      </c>
+      <c r="G91" s="1">
+        <v>1</v>
+      </c>
+      <c r="H91" s="1">
+        <v>0</v>
+      </c>
+      <c r="I91" s="1">
+        <v>0</v>
+      </c>
+      <c r="J91" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E92" s="1">
+        <v>60</v>
+      </c>
+      <c r="F92" s="1">
+        <v>1</v>
+      </c>
+      <c r="G92" s="1">
+        <v>0</v>
+      </c>
+      <c r="H92" s="1">
+        <v>0</v>
+      </c>
+      <c r="I92" s="1">
+        <v>0</v>
+      </c>
+      <c r="J92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E93" s="1">
+        <v>60</v>
+      </c>
+      <c r="F93" s="1">
+        <v>1</v>
+      </c>
+      <c r="G93" s="1">
+        <v>0</v>
+      </c>
+      <c r="H93" s="1">
+        <v>0</v>
+      </c>
+      <c r="I93" s="1">
+        <v>0</v>
+      </c>
+      <c r="J93" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:I43">
@@ -3973,6 +4383,9 @@
   </sortState>
   <hyperlinks>
     <hyperlink ref="C76" r:id="rId1" xr:uid="{D935FA78-FA00-4B71-A864-199CB53BF8F4}"/>
+    <hyperlink ref="C87" r:id="rId2" location="keyWordSearch=Python" xr:uid="{C957A0A2-4937-4544-AAC7-D50CCE88DC33}"/>
+    <hyperlink ref="C89" r:id="rId3" xr:uid="{777C39A2-DAF8-46B2-8961-BBC4FC7074E3}"/>
+    <hyperlink ref="C15" r:id="rId4" xr:uid="{30D7857E-D9CA-405D-B2B3-C50A75A14DE0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3991,20 +4404,20 @@
     <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4012,7 +4425,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4020,7 +4433,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4028,7 +4441,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -4050,11 +4463,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4062,7 +4475,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4070,7 +4483,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4078,7 +4491,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4086,7 +4499,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4094,7 +4507,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4102,7 +4515,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4110,7 +4523,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4118,7 +4531,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4126,7 +4539,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4134,7 +4547,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -4156,11 +4569,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>141</v>
+      <c r="A1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4168,7 +4581,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -4176,7 +4589,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -4184,7 +4597,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -4192,7 +4605,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -4200,7 +4613,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -4208,7 +4621,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -4216,7 +4629,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4224,7 +4637,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -4232,7 +4645,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4240,7 +4653,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -4248,7 +4661,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4256,7 +4669,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -4264,7 +4677,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -4272,7 +4685,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -4280,7 +4693,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>